<commit_message>
Update after a while
</commit_message>
<xml_diff>
--- a/obsidian-notes/spreadsheets/area.xlsx
+++ b/obsidian-notes/spreadsheets/area.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sharm\iCloudDrive\iCloud~md~obsidian\Ishan's notes\Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C6718E-35F4-46F7-BAD0-EC891325F105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6B907D-3ADF-4D44-9AD0-F65A08D16431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-48" yWindow="-48" windowWidth="20832" windowHeight="12336" activeTab="1" xr2:uid="{94B94BC7-FBC8-4BAC-A974-CA3E4662C848}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" activeTab="3" xr2:uid="{94B94BC7-FBC8-4BAC-A974-CA3E4662C848}"/>
   </bookViews>
   <sheets>
     <sheet name="france" sheetId="1" r:id="rId1"/>
-    <sheet name="united states" sheetId="2" r:id="rId2"/>
-    <sheet name="buenaventura" sheetId="4" r:id="rId3"/>
+    <sheet name="batavian republic" sheetId="18" r:id="rId2"/>
+    <sheet name="united states" sheetId="2" r:id="rId3"/>
+    <sheet name="buenaventura" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="252">
   <si>
     <t>OTL Metro France</t>
   </si>
@@ -783,6 +783,18 @@
   </si>
   <si>
     <t>Clinton[9]</t>
+  </si>
+  <si>
+    <t>Comancheria</t>
+  </si>
+  <si>
+    <t>Northern March</t>
+  </si>
+  <si>
+    <t>OTL Netherlands</t>
+  </si>
+  <si>
+    <t>East Frisia</t>
   </si>
 </sst>
 </file>
@@ -1231,24 +1243,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F489DD57-E97E-46C5-91B6-044FDCA9CA47}">
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83984375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="28" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="28"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1260,7 +1272,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1272,7 +1284,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1284,7 +1296,7 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1295,7 +1307,7 @@
         <v>875.8</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -1306,7 +1318,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E7" t="s">
         <v>5</v>
       </c>
@@ -1317,7 +1329,7 @@
         <v>2570</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="I8" t="s">
@@ -1330,7 +1342,7 @@
         <v>626.79999999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="I9" t="s">
@@ -1343,7 +1355,7 @@
         <v>642.37</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="I10" t="s">
@@ -1356,7 +1368,7 @@
         <v>989.05</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="I11" t="s">
@@ -1369,7 +1381,7 @@
         <v>782.18</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="I12" t="s">
@@ -1382,7 +1394,7 @@
         <v>24.12</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="I13" t="s">
@@ -1395,7 +1407,7 @@
         <v>26.34</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="I14" s="3" t="s">
@@ -1410,7 +1422,7 @@
         <v>26.3125</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E15" t="s">
         <v>6</v>
       </c>
@@ -1423,7 +1435,7 @@
         <v>16737.037499999999</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="I16" t="s">
@@ -1438,7 +1450,7 @@
         <v>2644.9050000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="I17" t="s">
@@ -1453,7 +1465,7 @@
         <v>4418.826</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E18" s="3" t="s">
         <v>8</v>
       </c>
@@ -1466,7 +1478,7 @@
         <v>7063.7309999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1479,7 +1491,7 @@
         <v>26370.768499999998</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E20" t="s">
         <v>9</v>
       </c>
@@ -1490,7 +1502,7 @@
         <v>282.49</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E21" t="s">
         <v>10</v>
       </c>
@@ -1501,7 +1513,7 @@
         <v>3211.94</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E22" t="s">
         <v>11</v>
       </c>
@@ -1512,7 +1524,7 @@
         <v>5224.49</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E23" t="s">
         <v>12</v>
       </c>
@@ -1523,7 +1535,7 @@
         <v>1671.42</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E24" t="s">
         <v>13</v>
       </c>
@@ -1534,7 +1546,7 @@
         <v>802.24</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E25" t="s">
         <v>14</v>
       </c>
@@ -1545,7 +1557,7 @@
         <v>838.51</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E26" t="s">
         <v>15</v>
       </c>
@@ -1556,7 +1568,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E27" t="s">
         <v>16</v>
       </c>
@@ -1567,7 +1579,7 @@
         <v>89.55</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E28" s="3" t="s">
         <v>17</v>
       </c>
@@ -1580,7 +1592,7 @@
         <v>42.029999999999994</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
@@ -1593,7 +1605,7 @@
         <v>12703.67</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A30" s="4" t="s">
         <v>18</v>
       </c>
@@ -1606,7 +1618,7 @@
         <v>627130.63850000012</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E31" t="s">
         <v>20</v>
       </c>
@@ -1617,7 +1629,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E32" s="3" t="s">
         <v>77</v>
       </c>
@@ -1628,7 +1640,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="3" t="s">
         <v>21</v>
       </c>
@@ -1641,7 +1653,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A34" s="4" t="s">
         <v>22</v>
       </c>
@@ -1654,8 +1666,8 @@
         <v>627872.63850000012</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>63</v>
       </c>
@@ -1663,7 +1675,7 @@
         <v>131324241</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>64</v>
       </c>
@@ -1676,7 +1688,7 @@
         <v>209.15745160314066</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>73</v>
       </c>
@@ -1687,7 +1699,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>72</v>
       </c>
@@ -1700,7 +1712,7 @@
         <v>47802023.723999985</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>75</v>
       </c>
@@ -1712,7 +1724,7 @@
         <v>20880554.319000002</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>71</v>
       </c>
@@ -1724,7 +1736,7 @@
         <v>14183018.027999999</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>70</v>
       </c>
@@ -1736,7 +1748,7 @@
         <v>9980642.3159999996</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>69</v>
       </c>
@@ -1748,7 +1760,7 @@
         <v>6828860.5319999997</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>68</v>
       </c>
@@ -1760,7 +1772,7 @@
         <v>4071051.4709999999</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>67</v>
       </c>
@@ -1773,7 +1785,7 @@
       </c>
       <c r="G47" s="13"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>66</v>
       </c>
@@ -1785,7 +1797,7 @@
         <v>6303563.568</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>65</v>
       </c>
@@ -1797,7 +1809,7 @@
         <v>2757809.0610000002</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>22</v>
       </c>
@@ -1818,29 +1830,94 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02846DC9-4F52-48FF-970A-2B60E31B58CA}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="1">
+        <v>41865</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B2" s="1">
+        <v>3142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <f>france!C5</f>
+        <v>875.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D4" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="6">
+        <f>france!C6</f>
+        <v>2210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3">
+        <f>-SUM(E3:E4)</f>
+        <v>-3085.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1">
+        <f>SUM(B1:B5)</f>
+        <v>41921.199999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C745E12-030D-4421-A6DC-982053D4A77E}">
   <dimension ref="A1:L227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.26171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.15625" customWidth="1"/>
+    <col min="4" max="5" width="9.578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.15625" customWidth="1"/>
+    <col min="11" max="11" width="12.15625" customWidth="1"/>
+    <col min="12" max="12" width="10.83984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E2" t="s">
         <v>24</v>
       </c>
@@ -1851,7 +1928,7 @@
         <v>469616</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E3" t="s">
         <v>25</v>
       </c>
@@ -1862,7 +1939,7 @@
         <v>780541</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E4" t="s">
         <v>26</v>
       </c>
@@ -1873,7 +1950,7 @@
         <v>758842</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E5" s="3" t="s">
         <v>27</v>
       </c>
@@ -1884,7 +1961,7 @@
         <v>475014</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1897,7 +1974,7 @@
         <v>2484013</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E7" t="s">
         <v>29</v>
       </c>
@@ -1910,7 +1987,7 @@
         <v>1134615</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="I8" t="s">
         <v>48</v>
       </c>
@@ -1921,7 +1998,7 @@
         <v>4770</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="I9" t="s">
         <v>49</v>
       </c>
@@ -1932,7 +2009,7 @@
         <v>5310</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="I10" s="3" t="s">
         <v>50</v>
       </c>
@@ -1943,7 +2020,7 @@
         <v>4710</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E11" t="s">
         <v>30</v>
       </c>
@@ -1956,7 +2033,7 @@
         <v>166248</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E12" t="s">
         <v>31</v>
       </c>
@@ -1967,7 +2044,7 @@
         <v>303448.18699999998</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="I13" t="s">
@@ -1980,7 +2057,7 @@
         <v>10920</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="I14" t="s">
@@ -1993,7 +2070,7 @@
         <v>12780</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="I15" t="s">
@@ -2006,7 +2083,7 @@
         <v>10610</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="I16" t="s">
@@ -2019,7 +2096,7 @@
         <v>5410</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="I17" t="s">
@@ -2032,7 +2109,7 @@
         <v>27170</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="I18" s="3" t="s">
@@ -2045,7 +2122,7 @@
         <v>19050</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E19" t="s">
         <v>32</v>
       </c>
@@ -2058,7 +2135,7 @@
         <v>167660</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E20" t="s">
         <v>33</v>
       </c>
@@ -2071,7 +2148,7 @@
         <v>134800.5</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E21" s="3" t="s">
         <v>34</v>
       </c>
@@ -2084,7 +2161,7 @@
         <v>193590.3636364</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -2097,7 +2174,7 @@
         <v>2100362.0506364</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="I23" t="s">
@@ -2110,7 +2187,7 @@
         <v>6920</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="I24" t="s">
@@ -2123,7 +2200,7 @@
         <v>5650</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="I25" t="s">
@@ -2136,7 +2213,7 @@
         <v>5760</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="I26" s="3" t="s">
@@ -2151,7 +2228,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E27" t="s">
         <v>36</v>
       </c>
@@ -2164,7 +2241,7 @@
         <v>19690</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E28" s="3" t="s">
         <v>37</v>
       </c>
@@ -2175,7 +2252,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -2188,7 +2265,7 @@
         <v>19690.41</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>61</v>
       </c>
@@ -2199,7 +2276,7 @@
         <v>12981.02</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>62</v>
       </c>
@@ -2210,7 +2287,7 @@
         <v>148.12100000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A32" s="4" t="s">
         <v>22</v>
       </c>
@@ -2223,17 +2300,17 @@
         <v>4617194.6016363995</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>126</v>
       </c>
       <c r="B34" s="12">
         <f>C84^(1/3)</f>
-        <v>680.86395376748942</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+        <v>680.66903588389926</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>121</v>
       </c>
@@ -2241,28 +2318,28 @@
         <v>675</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>122</v>
       </c>
       <c r="B36" s="15">
         <f>C84/B35</f>
-        <v>467602.96296296298</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+        <v>467201.48148148146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>120</v>
       </c>
       <c r="B37" s="15">
         <f>B36+C37</f>
-        <v>469602.96296296298</v>
+        <v>469201.48148148146</v>
       </c>
       <c r="C37">
         <v>2000</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>127</v>
       </c>
@@ -2273,7 +2350,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>128</v>
       </c>
@@ -2296,7 +2373,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="22">
         <v>1</v>
       </c>
@@ -2309,7 +2386,7 @@
       <c r="D41" s="23"/>
       <c r="E41" s="24">
         <f t="shared" ref="E41:E82" si="0">C41/$B$37</f>
-        <v>3.2346473932273754</v>
+        <v>3.2374151829270219</v>
       </c>
       <c r="F41" s="25">
         <f t="shared" ref="F41:F83" si="1">FLOOR(E41,1)</f>
@@ -2334,7 +2411,7 @@
         <v>527850</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <v>2</v>
       </c>
@@ -2347,7 +2424,7 @@
       <c r="D42" s="1"/>
       <c r="E42" s="12">
         <f t="shared" si="0"/>
-        <v>33.291953486317837</v>
+        <v>33.320440401501685</v>
       </c>
       <c r="F42" s="15">
         <f t="shared" si="1"/>
@@ -2370,7 +2447,7 @@
         <v>8036100</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="22">
         <v>3</v>
       </c>
@@ -2383,7 +2460,7 @@
       <c r="D43" s="23"/>
       <c r="E43" s="24">
         <f t="shared" si="0"/>
-        <v>25.845237268993191</v>
+        <v>25.867352254894843</v>
       </c>
       <c r="F43" s="25">
         <f t="shared" si="1"/>
@@ -2408,7 +2485,7 @@
         <v>4799400</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <v>4</v>
       </c>
@@ -2421,7 +2498,7 @@
       <c r="D44" s="1"/>
       <c r="E44" s="12">
         <f t="shared" si="0"/>
-        <v>24.512196276129242</v>
+        <v>24.533170619271196</v>
       </c>
       <c r="F44" s="15">
         <f t="shared" si="1"/>
@@ -2444,7 +2521,7 @@
         <v>6331333.333333333</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="22">
         <v>5</v>
       </c>
@@ -2457,7 +2534,7 @@
       <c r="D45" s="23"/>
       <c r="E45" s="24">
         <f t="shared" si="0"/>
-        <v>7.7640055271277228</v>
+        <v>7.7706489512520882</v>
       </c>
       <c r="F45" s="25">
         <f t="shared" si="1"/>
@@ -2482,7 +2559,7 @@
         <v>2378500</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
         <v>6</v>
       </c>
@@ -2495,7 +2572,7 @@
       <c r="D46" s="1"/>
       <c r="E46" s="12">
         <f t="shared" si="0"/>
-        <v>18.490087765235881</v>
+        <v>18.505909172715821</v>
       </c>
       <c r="F46" s="15">
         <f t="shared" si="1"/>
@@ -2507,7 +2584,7 @@
       </c>
       <c r="H46">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K46" s="11">
         <f>K99*0.8</f>
@@ -2518,7 +2595,7 @@
         <v>5176800</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="22">
         <v>7</v>
       </c>
@@ -2531,7 +2608,7 @@
       <c r="D47" s="23"/>
       <c r="E47" s="24">
         <f t="shared" si="0"/>
-        <v>10.172423039794058</v>
+        <v>10.181127273760621</v>
       </c>
       <c r="F47" s="25">
         <f t="shared" si="1"/>
@@ -2556,7 +2633,7 @@
         <v>3775055.5555555555</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
         <v>8</v>
       </c>
@@ -2569,7 +2646,7 @@
       <c r="D48" s="1"/>
       <c r="E48" s="12">
         <f t="shared" si="0"/>
-        <v>19.416402193184471</v>
+        <v>19.433016219834489</v>
       </c>
       <c r="F48" s="15">
         <f t="shared" si="1"/>
@@ -2592,7 +2669,7 @@
         <v>6606300</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="22">
         <v>9</v>
       </c>
@@ -2605,7 +2682,7 @@
       <c r="D49" s="23"/>
       <c r="E49" s="24">
         <f t="shared" si="0"/>
-        <v>3.2878838546037312</v>
+        <v>3.2906971971292442</v>
       </c>
       <c r="F49" s="25">
         <f t="shared" si="1"/>
@@ -2630,7 +2707,7 @@
         <v>485325</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
         <v>10</v>
       </c>
@@ -2638,35 +2715,35 @@
         <v>87</v>
       </c>
       <c r="C50" s="1">
-        <v>17041000</v>
+        <v>17541000</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="12">
         <f t="shared" si="0"/>
-        <v>36.288101532579134</v>
+        <v>37.3847924448472</v>
       </c>
       <c r="F50" s="15">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G50">
         <f t="shared" si="3"/>
-        <v>36.496575181789318</v>
+        <v>37.49666651850535</v>
       </c>
       <c r="H50">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K50" s="11">
         <f>K100+K102*(2.5/9)</f>
         <v>10099055.555555556</v>
       </c>
       <c r="L50" s="11">
-        <f>E183+E185*(2.5/9)+E200*0.8</f>
-        <v>14051055.555555556</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+        <f>E183+E185*(3/9)+E200*0.8</f>
+        <v>14555666.666666666</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="22">
         <v>11</v>
       </c>
@@ -2679,7 +2756,7 @@
       <c r="D51" s="23"/>
       <c r="E51" s="24">
         <f t="shared" si="0"/>
-        <v>85.687278772927172</v>
+        <v>85.760598779328788</v>
       </c>
       <c r="F51" s="25">
         <f t="shared" si="1"/>
@@ -2704,7 +2781,7 @@
         <v>24289750</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
         <v>12</v>
       </c>
@@ -2717,7 +2794,7 @@
       <c r="D52" s="1"/>
       <c r="E52" s="12">
         <f t="shared" si="0"/>
-        <v>24.512196276129242</v>
+        <v>24.533170619271196</v>
       </c>
       <c r="F52" s="15">
         <f t="shared" si="1"/>
@@ -2740,7 +2817,7 @@
         <v>4383000</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="22">
         <v>13</v>
       </c>
@@ -2753,7 +2830,7 @@
       <c r="D53" s="23"/>
       <c r="E53" s="24">
         <f t="shared" si="0"/>
-        <v>2.3381453836495445</v>
+        <v>2.3401460637615998</v>
       </c>
       <c r="F53" s="25">
         <f t="shared" si="1"/>
@@ -2778,7 +2855,7 @@
         <v>808875</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A54">
         <v>14</v>
       </c>
@@ -2791,7 +2868,7 @@
       <c r="D54" s="1"/>
       <c r="E54" s="12">
         <f t="shared" si="0"/>
-        <v>1.3777596204200868</v>
+        <v>1.3789385275535111</v>
       </c>
       <c r="F54" s="15">
         <f t="shared" si="1"/>
@@ -2806,7 +2883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="22">
         <v>15</v>
       </c>
@@ -2819,7 +2896,7 @@
       <c r="D55" s="23"/>
       <c r="E55" s="24">
         <f t="shared" si="0"/>
-        <v>20.061628105065903</v>
+        <v>20.078794231965421</v>
       </c>
       <c r="F55" s="25">
         <f t="shared" si="1"/>
@@ -2844,7 +2921,7 @@
         <v>5227300</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A56">
         <v>16</v>
       </c>
@@ -2858,7 +2935,7 @@
       <c r="D56" s="1"/>
       <c r="E56" s="12">
         <f t="shared" si="0"/>
-        <v>22.316724608968332</v>
+        <v>22.335820353571552</v>
       </c>
       <c r="F56" s="15">
         <f t="shared" si="1"/>
@@ -2881,7 +2958,7 @@
         <v>5558400</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="22">
         <v>17</v>
       </c>
@@ -2894,7 +2971,7 @@
       <c r="D57" s="23"/>
       <c r="E57" s="24">
         <f t="shared" si="0"/>
-        <v>49.948577521752021</v>
+        <v>49.991317005092974</v>
       </c>
       <c r="F57" s="25">
         <f t="shared" si="1"/>
@@ -2919,7 +2996,7 @@
         <v>15592000</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
         <v>18</v>
       </c>
@@ -2932,7 +3009,7 @@
       <c r="D58" s="1"/>
       <c r="E58" s="12">
         <f t="shared" si="0"/>
-        <v>19.382330857903604</v>
+        <v>19.398915730745063</v>
       </c>
       <c r="F58" s="15">
         <f t="shared" si="1"/>
@@ -2955,7 +3032,7 @@
         <v>6915700</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="22">
         <v>19</v>
       </c>
@@ -2968,7 +3045,7 @@
       <c r="D59" s="23"/>
       <c r="E59" s="24">
         <f t="shared" si="0"/>
-        <v>11.290388728697529</v>
+        <v>11.300049572007287</v>
       </c>
       <c r="F59" s="25">
         <f t="shared" si="1"/>
@@ -2993,7 +3070,7 @@
         <v>2790900</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A60">
         <v>20</v>
       </c>
@@ -3006,7 +3083,7 @@
       <c r="D60" s="1"/>
       <c r="E60" s="12">
         <f t="shared" si="0"/>
-        <v>14.486705869733928</v>
+        <v>14.499101704708711</v>
       </c>
       <c r="F60" s="15">
         <f t="shared" si="1"/>
@@ -3018,7 +3095,7 @@
       </c>
       <c r="H60">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K60" s="11">
         <f>K96*(1/3)+K124+K115*0.1+K122*0.7</f>
@@ -3029,7 +3106,7 @@
         <v>5776966.666666666</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="22">
         <v>21</v>
       </c>
@@ -3042,7 +3119,7 @@
       <c r="D61" s="23"/>
       <c r="E61" s="24">
         <f t="shared" si="0"/>
-        <v>3.1963171410363995</v>
+        <v>3.1990521327014219</v>
       </c>
       <c r="F61" s="25">
         <f t="shared" si="1"/>
@@ -3067,7 +3144,7 @@
         <v>532300</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A62">
         <v>22</v>
       </c>
@@ -3080,7 +3157,7 @@
       <c r="D62" s="1"/>
       <c r="E62" s="12">
         <f t="shared" si="0"/>
-        <v>24.729401038544776</v>
+        <v>24.750561237216264</v>
       </c>
       <c r="F62" s="15">
         <f t="shared" si="1"/>
@@ -3103,7 +3180,7 @@
         <v>9099400</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="22">
         <v>23</v>
       </c>
@@ -3116,7 +3193,7 @@
       <c r="D63" s="23"/>
       <c r="E63" s="24">
         <f t="shared" si="0"/>
-        <v>18.911720539336617</v>
+        <v>18.92790272519742</v>
       </c>
       <c r="F63" s="25">
         <f t="shared" si="1"/>
@@ -3141,7 +3218,7 @@
         <v>2493400</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A64">
         <v>24</v>
       </c>
@@ -3154,7 +3231,7 @@
       <c r="D64" s="1"/>
       <c r="E64" s="12">
         <f t="shared" si="0"/>
-        <v>47.28036607756907</v>
+        <v>47.320822453277593</v>
       </c>
       <c r="F64" s="15">
         <f t="shared" si="1"/>
@@ -3177,7 +3254,7 @@
         <v>13566666.666666664</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="22">
         <v>25</v>
       </c>
@@ -3190,7 +3267,7 @@
       <c r="D65" s="23"/>
       <c r="E65" s="24">
         <f t="shared" si="0"/>
-        <v>15.532269971165555</v>
+        <v>15.545560463640355</v>
       </c>
       <c r="F65" s="25">
         <f t="shared" si="1"/>
@@ -3215,7 +3292,7 @@
         <v>3499400</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A66">
         <v>26</v>
       </c>
@@ -3228,7 +3305,7 @@
       <c r="D66" s="1"/>
       <c r="E66" s="12">
         <f t="shared" si="0"/>
-        <v>7.5084705125212157</v>
+        <v>7.5148952830814215</v>
       </c>
       <c r="F66" s="15">
         <f t="shared" si="1"/>
@@ -3251,7 +3328,7 @@
         <v>876200</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="22">
         <v>27</v>
       </c>
@@ -3264,7 +3341,7 @@
       <c r="D67" s="23"/>
       <c r="E67" s="24">
         <f t="shared" si="0"/>
-        <v>18.232423292174317</v>
+        <v>18.248024223977065</v>
       </c>
       <c r="F67" s="25">
         <f t="shared" si="1"/>
@@ -3289,7 +3366,7 @@
         <v>5651900</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A68">
         <v>28</v>
       </c>
@@ -3302,7 +3379,7 @@
       <c r="D68" s="1"/>
       <c r="E68" s="12">
         <f t="shared" si="0"/>
-        <v>7.3317254607517146</v>
+        <v>7.337998995930044</v>
       </c>
       <c r="F68" s="15">
         <f t="shared" si="1"/>
@@ -3325,7 +3402,7 @@
         <v>1980666.6666666665</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="22">
         <v>29</v>
       </c>
@@ -3338,7 +3415,7 @@
       <c r="D69" s="23"/>
       <c r="E69" s="24">
         <f t="shared" si="0"/>
-        <v>11.364919774624425</v>
+        <v>11.374644391890399</v>
       </c>
       <c r="F69" s="25">
         <f t="shared" si="1"/>
@@ -3363,7 +3440,7 @@
         <v>3961333.333333333</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A70">
         <v>30</v>
       </c>
@@ -3376,7 +3453,7 @@
       <c r="D70" s="1"/>
       <c r="E70" s="12">
         <f t="shared" si="0"/>
-        <v>5.3960477251074188</v>
+        <v>5.4006649595372442</v>
       </c>
       <c r="F70" s="15">
         <f t="shared" si="1"/>
@@ -3395,7 +3472,7 @@
         <v>1248000</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="22">
         <v>31</v>
       </c>
@@ -3408,7 +3485,7 @@
       <c r="D71" s="23"/>
       <c r="E71" s="24">
         <f t="shared" si="0"/>
-        <v>14.737981967430327</v>
+        <v>14.750592811743198</v>
       </c>
       <c r="F71" s="25">
         <f t="shared" si="1"/>
@@ -3433,7 +3510,7 @@
         <v>5658666.666666666</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A72">
         <v>32</v>
       </c>
@@ -3446,7 +3523,7 @@
       <c r="D72" s="1"/>
       <c r="E72" s="12">
         <f t="shared" si="0"/>
-        <v>2.2827794638181347</v>
+        <v>2.2847327689912889</v>
       </c>
       <c r="F72" s="15">
         <f t="shared" si="1"/>
@@ -3461,7 +3538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="22">
         <v>33</v>
       </c>
@@ -3474,7 +3551,7 @@
       <c r="D73" s="23"/>
       <c r="E73" s="24">
         <f t="shared" si="0"/>
-        <v>10.459899931226378</v>
+        <v>10.468850150452621</v>
       </c>
       <c r="F73" s="25">
         <f t="shared" si="1"/>
@@ -3499,7 +3576,7 @@
         <v>4428000</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A74">
         <v>34</v>
       </c>
@@ -3512,7 +3589,7 @@
       <c r="D74" s="1"/>
       <c r="E74" s="12">
         <f t="shared" si="0"/>
-        <v>3.5838785798562691</v>
+        <v>3.5869451960935996</v>
       </c>
       <c r="F74" s="15">
         <f t="shared" si="1"/>
@@ -3531,7 +3608,7 @@
         <v>670000</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="22">
         <v>35</v>
       </c>
@@ -3544,7 +3621,7 @@
       <c r="D75" s="23"/>
       <c r="E75" s="24">
         <f t="shared" si="0"/>
-        <v>3.036607756907332</v>
+        <v>3.0392060900947553</v>
       </c>
       <c r="F75" s="25">
         <f t="shared" si="1"/>
@@ -3566,7 +3643,7 @@
         <v>732600</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A76">
         <v>36</v>
       </c>
@@ -3579,7 +3656,7 @@
       <c r="D76" s="1"/>
       <c r="E76" s="12">
         <f t="shared" si="0"/>
-        <v>15.553564555716097</v>
+        <v>15.566873269321244</v>
       </c>
       <c r="F76" s="15">
         <f t="shared" si="1"/>
@@ -3598,7 +3675,7 @@
         <v>6788000</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="22">
         <v>37</v>
       </c>
@@ -3611,7 +3688,7 @@
       <c r="D77" s="23"/>
       <c r="E77" s="24">
         <f t="shared" si="0"/>
-        <v>6.8163965146285905</v>
+        <v>6.8222290984525324</v>
       </c>
       <c r="F77" s="25">
         <f t="shared" si="1"/>
@@ -3636,7 +3713,7 @@
         <v>1648666.6666666665</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A78">
         <v>38</v>
       </c>
@@ -3649,7 +3726,7 @@
       <c r="D78" s="1"/>
       <c r="E78" s="12">
         <f t="shared" si="0"/>
-        <v>2.2742616299979179</v>
+        <v>2.2762076467189329</v>
       </c>
       <c r="F78" s="15">
         <f t="shared" si="1"/>
@@ -3664,7 +3741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="22">
         <v>39</v>
       </c>
@@ -3672,25 +3749,25 @@
         <v>112</v>
       </c>
       <c r="C79" s="23">
-        <f>4303000</f>
-        <v>4303000</v>
+        <f>3532000</f>
+        <v>3532000</v>
       </c>
       <c r="D79" s="23"/>
       <c r="E79" s="24">
         <f t="shared" si="0"/>
-        <v>9.1630597320983522</v>
+        <v>7.5276829664899552</v>
       </c>
       <c r="F79" s="25">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G79" s="22">
         <f t="shared" si="3"/>
-        <v>9.4868329805051381</v>
+        <v>7.4833147735478827</v>
       </c>
       <c r="H79" s="22">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I79" s="22"/>
       <c r="J79" s="22"/>
@@ -3699,11 +3776,11 @@
         <v>4036888.8888888885</v>
       </c>
       <c r="L79" s="26">
-        <f>E185*(4/9)</f>
-        <v>4036888.8888888885</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+        <f>E185*(7/18)</f>
+        <v>3532277.777777778</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A80">
         <v>40</v>
       </c>
@@ -3716,7 +3793,7 @@
       <c r="D80" s="1"/>
       <c r="E80" s="12">
         <f t="shared" si="0"/>
-        <v>2.8343092036771802</v>
+        <v>2.8367344361263109</v>
       </c>
       <c r="F80" s="15">
         <f t="shared" si="1"/>
@@ -3731,7 +3808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="22">
         <v>41</v>
       </c>
@@ -3744,7 +3821,7 @@
       <c r="D81" s="23"/>
       <c r="E81" s="24">
         <f>C81/$B$37</f>
-        <v>6.6460398382242527</v>
+        <v>6.6517266530054213</v>
       </c>
       <c r="F81" s="25">
         <f>FLOOR(E81,1)</f>
@@ -3762,7 +3839,7 @@
       <c r="J81" s="22"/>
       <c r="K81" s="22"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A82">
         <v>42</v>
       </c>
@@ -3775,7 +3852,7 @@
       <c r="D82" s="1"/>
       <c r="E82" s="12">
         <f t="shared" si="0"/>
-        <v>0.92631442794859009</v>
+        <v>0.92710704711866654</v>
       </c>
       <c r="F82" s="15">
         <f t="shared" si="1"/>
@@ -3790,7 +3867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="22">
         <v>43</v>
       </c>
@@ -3803,7 +3880,7 @@
       <c r="D83" s="23"/>
       <c r="E83" s="24">
         <f>C83/$B$37</f>
-        <v>0.62180186887583522</v>
+        <v>0.62233392588195546</v>
       </c>
       <c r="F83" s="25">
         <f t="shared" si="1"/>
@@ -3821,42 +3898,42 @@
       <c r="J83" s="22"/>
       <c r="K83" s="22"/>
     </row>
-    <row r="84" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A84" s="4"/>
       <c r="B84" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C84" s="7">
         <f>SUM(C41:C83)</f>
-        <v>315632000</v>
+        <v>315361000</v>
       </c>
       <c r="D84" s="7"/>
       <c r="E84" s="7">
         <f>SUM(E41:E83)</f>
-        <v>672.12523108567655</v>
+        <v>672.12277123308002</v>
       </c>
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
       <c r="H84" s="7">
         <f>SUM(H41:H83)</f>
-        <v>670</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
         <v>64</v>
       </c>
       <c r="B86" s="12">
         <f>$C$84/B32</f>
-        <v>73.530055806280956</v>
+        <v>73.466923281304076</v>
       </c>
       <c r="C86" s="12">
         <f>$C$84/C32</f>
-        <v>68.360124974618898</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+        <v>68.301431325470134</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G94" t="s">
         <v>141</v>
       </c>
@@ -3873,7 +3950,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G95" s="20">
         <v>1</v>
       </c>
@@ -3890,7 +3967,7 @@
         <v>23785000</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G96" s="20">
         <v>2</v>
       </c>
@@ -3907,7 +3984,7 @@
         <v>15038000</v>
       </c>
     </row>
-    <row r="97" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G97" s="20">
         <v>3</v>
       </c>
@@ -3924,7 +4001,7 @@
         <v>10415000</v>
       </c>
     </row>
-    <row r="98" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G98" s="20">
         <v>4</v>
       </c>
@@ -3941,7 +4018,7 @@
         <v>7038000</v>
       </c>
     </row>
-    <row r="99" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G99" s="20">
         <v>5</v>
       </c>
@@ -3958,7 +4035,7 @@
         <v>6471000</v>
       </c>
     </row>
-    <row r="100" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G100" s="20">
         <v>6</v>
       </c>
@@ -3975,7 +4052,7 @@
         <v>7576000</v>
       </c>
     </row>
-    <row r="101" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G101" s="20">
         <v>7</v>
       </c>
@@ -3992,7 +4069,7 @@
         <v>6948000</v>
       </c>
     </row>
-    <row r="102" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G102" s="20">
         <v>8</v>
       </c>
@@ -4009,7 +4086,7 @@
         <v>9083000</v>
       </c>
     </row>
-    <row r="103" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G103" s="20">
         <v>9</v>
       </c>
@@ -4026,7 +4103,7 @@
         <v>6743000</v>
       </c>
     </row>
-    <row r="104" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G104" s="20">
         <v>10</v>
       </c>
@@ -4043,7 +4120,7 @@
         <v>5942000</v>
       </c>
     </row>
-    <row r="105" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G105" s="20">
         <v>11</v>
       </c>
@@ -4060,7 +4137,7 @@
         <v>4813000</v>
       </c>
     </row>
-    <row r="106" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G106" s="20">
         <v>12</v>
       </c>
@@ -4077,7 +4154,7 @@
         <v>4428000</v>
       </c>
     </row>
-    <row r="107" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G107" s="20">
         <v>13</v>
       </c>
@@ -4094,7 +4171,7 @@
         <v>3327000</v>
       </c>
     </row>
-    <row r="108" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G108" s="20">
         <v>14</v>
       </c>
@@ -4111,7 +4188,7 @@
         <v>3991000</v>
       </c>
     </row>
-    <row r="109" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G109" s="20">
         <v>15</v>
       </c>
@@ -4128,7 +4205,7 @@
         <v>15038000</v>
       </c>
     </row>
-    <row r="110" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G110" s="20">
         <v>16</v>
       </c>
@@ -4145,7 +4222,7 @@
         <v>1782000</v>
       </c>
     </row>
-    <row r="111" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G111" s="20">
         <v>17</v>
       </c>
@@ -4162,7 +4239,7 @@
         <v>3447000</v>
       </c>
     </row>
-    <row r="112" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G112" s="20">
         <v>18</v>
       </c>
@@ -4179,7 +4256,7 @@
         <v>4940000</v>
       </c>
     </row>
-    <row r="113" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G113" s="20">
         <v>19</v>
       </c>
@@ -4196,7 +4273,7 @@
         <v>23785000</v>
       </c>
     </row>
-    <row r="114" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G114" s="20">
         <v>20</v>
       </c>
@@ -4213,7 +4290,7 @@
         <v>6491000</v>
       </c>
     </row>
-    <row r="115" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G115" s="20">
         <v>21</v>
       </c>
@@ -4230,7 +4307,7 @@
         <v>2297000</v>
       </c>
     </row>
-    <row r="116" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G116" s="20">
         <v>22</v>
       </c>
@@ -4247,7 +4324,7 @@
         <v>2929000</v>
       </c>
     </row>
-    <row r="117" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G117" s="20">
         <v>23</v>
       </c>
@@ -4264,7 +4341,7 @@
         <v>4247000</v>
       </c>
     </row>
-    <row r="118" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G118" s="20">
         <v>24</v>
       </c>
@@ -4281,7 +4358,7 @@
         <v>2473000</v>
       </c>
     </row>
-    <row r="119" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G119" s="20">
         <v>25</v>
       </c>
@@ -4298,7 +4375,7 @@
         <v>1929000</v>
       </c>
     </row>
-    <row r="120" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G120" s="20">
         <v>26</v>
       </c>
@@ -4315,7 +4392,7 @@
         <v>5312000</v>
       </c>
     </row>
-    <row r="121" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G121" s="20">
         <v>27</v>
       </c>
@@ -4332,7 +4409,7 @@
         <v>1252000</v>
       </c>
     </row>
-    <row r="122" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G122" s="20">
         <v>28</v>
       </c>
@@ -4349,7 +4426,7 @@
         <v>1782000</v>
       </c>
     </row>
-    <row r="123" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G123" s="20">
         <v>29</v>
       </c>
@@ -4366,7 +4443,7 @@
         <v>2175000</v>
       </c>
     </row>
-    <row r="124" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G124" s="20">
         <v>30</v>
       </c>
@@ -4383,7 +4460,7 @@
         <v>1534000</v>
       </c>
     </row>
-    <row r="125" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G125" s="20">
         <v>31</v>
       </c>
@@ -4400,7 +4477,7 @@
         <v>2461000</v>
       </c>
     </row>
-    <row r="126" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G126" s="20">
         <v>32</v>
       </c>
@@ -4417,7 +4494,7 @@
         <v>1567000</v>
       </c>
     </row>
-    <row r="130" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G130" t="s">
         <v>141</v>
       </c>
@@ -4434,7 +4511,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="131" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G131">
         <v>1</v>
       </c>
@@ -4451,7 +4528,7 @@
         <v>23785000</v>
       </c>
     </row>
-    <row r="132" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G132">
         <v>2</v>
       </c>
@@ -4468,7 +4545,7 @@
         <v>15038000</v>
       </c>
     </row>
-    <row r="133" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G133">
         <v>3</v>
       </c>
@@ -4485,7 +4562,7 @@
         <v>10415000</v>
       </c>
     </row>
-    <row r="134" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G134">
         <v>4</v>
       </c>
@@ -4502,7 +4579,7 @@
         <v>7038000</v>
       </c>
     </row>
-    <row r="135" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G135">
         <v>5</v>
       </c>
@@ -4519,7 +4596,7 @@
         <v>6471000</v>
       </c>
     </row>
-    <row r="136" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G136">
         <v>6</v>
       </c>
@@ -4536,7 +4613,7 @@
         <v>7576000</v>
       </c>
     </row>
-    <row r="137" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G137">
         <v>7</v>
       </c>
@@ -4553,7 +4630,7 @@
         <v>6948000</v>
       </c>
     </row>
-    <row r="138" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G138">
         <v>8</v>
       </c>
@@ -4570,7 +4647,7 @@
         <v>9083000</v>
       </c>
     </row>
-    <row r="139" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G139">
         <v>9</v>
       </c>
@@ -4587,7 +4664,7 @@
         <v>6743000</v>
       </c>
     </row>
-    <row r="140" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G140">
         <v>10</v>
       </c>
@@ -4604,7 +4681,7 @@
         <v>5942000</v>
       </c>
     </row>
-    <row r="141" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G141">
         <v>11</v>
       </c>
@@ -4621,7 +4698,7 @@
         <v>4813000</v>
       </c>
     </row>
-    <row r="142" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G142">
         <v>12</v>
       </c>
@@ -4638,7 +4715,7 @@
         <v>4428000</v>
       </c>
     </row>
-    <row r="143" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G143">
         <v>13</v>
       </c>
@@ -4655,7 +4732,7 @@
         <v>3327000</v>
       </c>
     </row>
-    <row r="144" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G144">
         <v>14</v>
       </c>
@@ -4672,7 +4749,7 @@
         <v>3991000</v>
       </c>
     </row>
-    <row r="145" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G145">
         <v>15</v>
       </c>
@@ -4689,7 +4766,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="146" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G146">
         <v>16</v>
       </c>
@@ -4706,7 +4783,7 @@
         <v>2252000</v>
       </c>
     </row>
-    <row r="147" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G147">
         <v>17</v>
       </c>
@@ -4723,7 +4800,7 @@
         <v>3447000</v>
       </c>
     </row>
-    <row r="148" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G148">
         <v>18</v>
       </c>
@@ -4740,7 +4817,7 @@
         <v>6491000</v>
       </c>
     </row>
-    <row r="149" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G149">
         <v>19</v>
       </c>
@@ -4757,7 +4834,7 @@
         <v>5105000</v>
       </c>
     </row>
-    <row r="150" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G150">
         <v>20</v>
       </c>
@@ -4774,7 +4851,7 @@
         <v>1836000</v>
       </c>
     </row>
-    <row r="151" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G151">
         <v>21</v>
       </c>
@@ -4791,7 +4868,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="152" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G152">
         <v>22</v>
       </c>
@@ -4808,7 +4885,7 @@
         <v>4940000</v>
       </c>
     </row>
-    <row r="153" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G153">
         <v>23</v>
       </c>
@@ -4825,7 +4902,7 @@
         <v>2297000</v>
       </c>
     </row>
-    <row r="154" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G154">
         <v>24</v>
       </c>
@@ -4842,7 +4919,7 @@
         <v>2929000</v>
       </c>
     </row>
-    <row r="155" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G155">
         <v>25</v>
       </c>
@@ -4859,7 +4936,7 @@
         <v>4247000</v>
       </c>
     </row>
-    <row r="156" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G156">
         <v>26</v>
       </c>
@@ -4876,7 +4953,7 @@
         <v>3562000</v>
       </c>
     </row>
-    <row r="157" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G157">
         <v>27</v>
       </c>
@@ -4893,7 +4970,7 @@
         <v>3421000</v>
       </c>
     </row>
-    <row r="158" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G158">
         <v>28</v>
       </c>
@@ -4910,7 +4987,7 @@
         <v>2473000</v>
       </c>
     </row>
-    <row r="159" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G159">
         <v>29</v>
       </c>
@@ -4927,7 +5004,7 @@
         <v>2329000</v>
       </c>
     </row>
-    <row r="160" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G160">
         <v>30</v>
       </c>
@@ -4944,7 +5021,7 @@
         <v>1651000</v>
       </c>
     </row>
-    <row r="161" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G161">
         <v>31</v>
       </c>
@@ -4961,7 +5038,7 @@
         <v>2547000</v>
       </c>
     </row>
-    <row r="162" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G162">
         <v>32</v>
       </c>
@@ -4978,7 +5055,7 @@
         <v>5312000</v>
       </c>
     </row>
-    <row r="163" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G163">
         <v>33</v>
       </c>
@@ -4995,7 +5072,7 @@
         <v>1252000</v>
       </c>
     </row>
-    <row r="164" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G164">
         <v>34</v>
       </c>
@@ -5012,7 +5089,7 @@
         <v>1782000</v>
       </c>
     </row>
-    <row r="165" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G165">
         <v>35</v>
       </c>
@@ -5029,7 +5106,7 @@
         <v>2175000</v>
       </c>
     </row>
-    <row r="166" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G166">
         <v>36</v>
       </c>
@@ -5046,7 +5123,7 @@
         <v>2461000</v>
       </c>
     </row>
-    <row r="167" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G167">
         <v>37</v>
       </c>
@@ -5063,7 +5140,7 @@
         <v>1221000</v>
       </c>
     </row>
-    <row r="168" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G168">
         <v>38</v>
       </c>
@@ -5080,7 +5157,7 @@
         <v>1614000</v>
       </c>
     </row>
-    <row r="169" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G169">
         <v>39</v>
       </c>
@@ -5097,7 +5174,7 @@
         <v>1567000</v>
       </c>
     </row>
-    <row r="170" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G170">
         <v>40</v>
       </c>
@@ -5114,7 +5191,7 @@
         <v>1341000</v>
       </c>
     </row>
-    <row r="171" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G171">
         <v>41</v>
       </c>
@@ -5131,7 +5208,7 @@
         <v>1248000</v>
       </c>
     </row>
-    <row r="172" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G172">
         <v>42</v>
       </c>
@@ -5148,7 +5225,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="173" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G173">
         <v>43</v>
       </c>
@@ -5165,7 +5242,7 @@
         <v>1641000</v>
       </c>
     </row>
-    <row r="174" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G174">
         <v>44</v>
       </c>
@@ -5182,7 +5259,7 @@
         <v>1051000</v>
       </c>
     </row>
-    <row r="175" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="7:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G175">
         <v>45</v>
       </c>
@@ -5199,7 +5276,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" t="s">
         <v>141</v>
       </c>
@@ -5216,7 +5293,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A178">
         <v>1</v>
       </c>
@@ -5233,7 +5310,7 @@
         <v>23785000</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A179">
         <v>2</v>
       </c>
@@ -5250,7 +5327,7 @@
         <v>15038000</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A180">
         <v>3</v>
       </c>
@@ -5267,7 +5344,7 @@
         <v>10415000</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A181">
         <v>4</v>
       </c>
@@ -5284,7 +5361,7 @@
         <v>7038000</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A182">
         <v>5</v>
       </c>
@@ -5301,7 +5378,7 @@
         <v>6471000</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A183">
         <v>6</v>
       </c>
@@ -5318,7 +5395,7 @@
         <v>7576000</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A184">
         <v>7</v>
       </c>
@@ -5335,7 +5412,7 @@
         <v>6948000</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A185">
         <v>8</v>
       </c>
@@ -5352,7 +5429,7 @@
         <v>9083000</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A186">
         <v>9</v>
       </c>
@@ -5369,7 +5446,7 @@
         <v>6743000</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A187">
         <v>10</v>
       </c>
@@ -5386,7 +5463,7 @@
         <v>5942000</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A188">
         <v>11</v>
       </c>
@@ -5403,7 +5480,7 @@
         <v>4813000</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A189">
         <v>12</v>
       </c>
@@ -5420,7 +5497,7 @@
         <v>4428000</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A190">
         <v>13</v>
       </c>
@@ -5437,7 +5514,7 @@
         <v>3327000</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A191">
         <v>14</v>
       </c>
@@ -5454,7 +5531,7 @@
         <v>3991000</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A192">
         <v>15</v>
       </c>
@@ -5471,7 +5548,7 @@
         <v>5147000</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A193">
         <v>16</v>
       </c>
@@ -5488,7 +5565,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A194">
         <v>17</v>
       </c>
@@ -5505,7 +5582,7 @@
         <v>2252000</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A195">
         <v>18</v>
       </c>
@@ -5522,7 +5599,7 @@
         <v>3447000</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A196">
         <v>19</v>
       </c>
@@ -5539,7 +5616,7 @@
         <v>6291000</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A197">
         <v>20</v>
       </c>
@@ -5556,7 +5633,7 @@
         <v>4405000</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A198">
         <v>21</v>
       </c>
@@ -5573,7 +5650,7 @@
         <v>1836000</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A199">
         <v>22</v>
       </c>
@@ -5590,7 +5667,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A200">
         <v>23</v>
       </c>
@@ -5607,7 +5684,7 @@
         <v>4940000</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A201">
         <v>24</v>
       </c>
@@ -5624,7 +5701,7 @@
         <v>2297000</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A202">
         <v>25</v>
       </c>
@@ -5641,7 +5718,7 @@
         <v>2929000</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A203">
         <v>26</v>
       </c>
@@ -5658,7 +5735,7 @@
         <v>3562000</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A204">
         <v>27</v>
       </c>
@@ -5675,7 +5752,7 @@
         <v>3421000</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A205">
         <v>28</v>
       </c>
@@ -5692,7 +5769,7 @@
         <v>2473000</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A206">
         <v>29</v>
       </c>
@@ -5709,7 +5786,7 @@
         <v>2329000</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A207">
         <v>30</v>
       </c>
@@ -5726,7 +5803,7 @@
         <v>1651000</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A208">
         <v>31</v>
       </c>
@@ -5743,7 +5820,7 @@
         <v>2547000</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A209">
         <v>32</v>
       </c>
@@ -5760,7 +5837,7 @@
         <v>5312000</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A210">
         <v>33</v>
       </c>
@@ -5777,7 +5854,7 @@
         <v>1252000</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A211">
         <v>34</v>
       </c>
@@ -5794,7 +5871,7 @@
         <v>1782000</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A212">
         <v>35</v>
       </c>
@@ -5811,7 +5888,7 @@
         <v>2175000</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A213">
         <v>36</v>
       </c>
@@ -5828,7 +5905,7 @@
         <v>2461000</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A214">
         <v>37</v>
       </c>
@@ -5845,7 +5922,7 @@
         <v>1221000</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A215">
         <v>38</v>
       </c>
@@ -5862,7 +5939,7 @@
         <v>1814000</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A216">
         <v>39</v>
       </c>
@@ -5879,7 +5956,7 @@
         <v>1567000</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A217">
         <v>40</v>
       </c>
@@ -5896,7 +5973,7 @@
         <v>1341000</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A218">
         <v>41</v>
       </c>
@@ -5913,7 +5990,7 @@
         <v>1248000</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A219">
         <v>42</v>
       </c>
@@ -5930,7 +6007,7 @@
         <v>1638000</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A220">
         <v>43</v>
       </c>
@@ -5947,7 +6024,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A221">
         <v>44</v>
       </c>
@@ -5964,7 +6041,7 @@
         <v>1641000</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A222">
         <v>45</v>
       </c>
@@ -5981,7 +6058,7 @@
         <v>1051000</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A223">
         <v>46</v>
       </c>
@@ -5998,7 +6075,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A224">
         <v>47</v>
       </c>
@@ -6015,7 +6092,7 @@
         <v>993000</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A225">
         <v>48</v>
       </c>
@@ -6032,7 +6109,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A226">
         <v>49</v>
       </c>
@@ -6049,7 +6126,7 @@
         <v>934000</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A227">
         <v>50</v>
       </c>
@@ -6072,30 +6149,30 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63D63CD-E558-4E85-B35D-432437BFD9B4}">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.83984375" customWidth="1"/>
+    <col min="4" max="4" width="10.41796875" customWidth="1"/>
+    <col min="5" max="5" width="10.578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83984375" customWidth="1"/>
+    <col min="11" max="11" width="10.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>131</v>
       </c>
@@ -6103,7 +6180,7 @@
         <v>1054549</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="D4" t="s">
         <v>132</v>
       </c>
@@ -6111,7 +6188,7 @@
         <v>9833520</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="D5" t="s">
         <v>133</v>
       </c>
@@ -6120,7 +6197,7 @@
         <v>4617194.6016363995</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G6" t="s">
         <v>134</v>
       </c>
@@ -6129,7 +6206,7 @@
         <v>77351.813000000024</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G7" t="s">
         <v>136</v>
       </c>
@@ -6138,7 +6215,7 @@
         <v>224595</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G8" t="s">
         <v>135</v>
       </c>
@@ -6146,7 +6223,7 @@
         <v>254806</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G9" t="s">
         <v>137</v>
       </c>
@@ -6155,7 +6232,7 @@
         <v>165137</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="D10" t="s">
         <v>138</v>
       </c>
@@ -6164,7 +6241,7 @@
         <v>721889.81300000008</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="D11" t="s">
         <v>140</v>
       </c>
@@ -6173,7 +6250,7 @@
         <v>13129.141</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
         <v>139</v>
       </c>
@@ -6182,7 +6259,7 @@
         <v>4481306.4443636006</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A13" s="17" t="s">
         <v>22</v>
       </c>
@@ -6191,10 +6268,10 @@
         <v>5535855.4443636006</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" t="s">
-        <v>129</v>
+        <v>174</v>
       </c>
       <c r="C15" t="s">
         <v>63</v>
@@ -6203,20 +6280,26 @@
         <v>173</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>1</v>
+      </c>
       <c r="B16" t="s">
         <v>177</v>
       </c>
       <c r="C16" s="1">
-        <f>K16+2000000</f>
+        <f>K16+1800000</f>
+        <v>13846000</v>
+      </c>
+      <c r="K16" s="1">
+        <f>E34</f>
         <v>12046000</v>
       </c>
-      <c r="K16" s="1">
-        <f>E32</f>
-        <v>10046000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>2</v>
+      </c>
       <c r="B17" t="s">
         <v>185</v>
       </c>
@@ -6225,11 +6308,14 @@
         <v>6602000</v>
       </c>
       <c r="K17" s="1">
-        <f>E36</f>
+        <f>E38</f>
         <v>4602000</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>3</v>
+      </c>
       <c r="B18" t="s">
         <v>179</v>
       </c>
@@ -6238,11 +6324,14 @@
         <v>11286000</v>
       </c>
       <c r="K18" s="1">
-        <f>E33</f>
+        <f>E35</f>
         <v>7524000</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>4</v>
+      </c>
       <c r="B19" t="s">
         <v>183</v>
       </c>
@@ -6251,11 +6340,14 @@
         <v>11924000</v>
       </c>
       <c r="K19" s="1">
-        <f>E35</f>
+        <f>E37</f>
         <v>4924000</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>5</v>
+      </c>
       <c r="B20" t="s">
         <v>194</v>
       </c>
@@ -6264,276 +6356,318 @@
       </c>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>6</v>
+      </c>
       <c r="B21" t="s">
+        <v>248</v>
+      </c>
+      <c r="C21" s="1">
+        <v>221000</v>
+      </c>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>249</v>
+      </c>
+      <c r="C22" s="1">
+        <v>628000</v>
+      </c>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
         <v>187</v>
       </c>
-      <c r="C21" s="11">
-        <f>K21*1.5</f>
-        <v>14124000</v>
-      </c>
-      <c r="K21" s="1">
-        <f>SUM(E37:E39)+E41</f>
+      <c r="C23" s="11">
+        <f>K23*1.5-SUM(C21:C22)</f>
+        <v>13275000</v>
+      </c>
+      <c r="K23" s="1">
+        <f>SUM(E39:E41)+E43</f>
         <v>9416000</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>9</v>
+      </c>
+      <c r="B24" t="s">
         <v>181</v>
       </c>
-      <c r="C22" s="11">
-        <f>K22+1500000</f>
+      <c r="C24" s="11">
+        <f>K24+1500000</f>
         <v>8893000</v>
       </c>
-      <c r="K22" s="1">
-        <f>E40+E34</f>
+      <c r="K24" s="1">
+        <f>E42+E36</f>
         <v>7393000</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
         <v>192</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C25" s="1">
         <v>2341000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
         <v>193</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C26" s="1">
         <v>1567000</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27">
+        <v>12</v>
+      </c>
+      <c r="B27" t="s">
         <v>195</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C27" s="1">
         <v>234000</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28">
+        <v>13</v>
+      </c>
+      <c r="B28" t="s">
         <v>196</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C28" s="1">
         <v>1624000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4" t="s">
+    <row r="29" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="5">
-        <f>SUM(C16:C26)</f>
-        <v>72162000</v>
-      </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="C29" s="5">
+        <f>SUM(C16:C28)</f>
+        <v>73962000</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+    </row>
+    <row r="30" spans="1:11" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="8">
-        <f>C27/B13</f>
-        <v>13.035383731609652</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B31" s="8">
+        <f>C29/B13</f>
+        <v>13.360536730652047</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
         <v>141</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B33" t="s">
         <v>142</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C33" t="s">
         <v>174</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D33" t="s">
         <v>63</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E33" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34">
         <v>1</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B34" t="s">
         <v>176</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C34" t="s">
         <v>177</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D34" s="1">
         <v>5221000</v>
       </c>
-      <c r="E32" s="1">
-        <v>10046000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="E34" s="1">
+        <v>12046000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35">
         <v>2</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B35" t="s">
         <v>178</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C35" t="s">
         <v>179</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D35" s="1">
         <v>3270000</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E35" s="1">
         <v>7524000</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36">
         <v>3</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B36" t="s">
         <v>180</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C36" t="s">
         <v>181</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D36" s="1">
         <v>2769000</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E36" s="1">
         <v>5435000</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37">
         <v>4</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B37" t="s">
         <v>182</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C37" t="s">
         <v>183</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D37" s="1">
         <v>2534000</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E37" s="1">
         <v>4924000</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38">
         <v>5</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B38" t="s">
         <v>184</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C38" t="s">
         <v>185</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D38" s="1">
         <v>2150000</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E38" s="1">
         <v>4602000</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39">
         <v>6</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B39" t="s">
         <v>186</v>
-      </c>
-      <c r="C37" t="s">
-        <v>187</v>
-      </c>
-      <c r="D37" s="1">
-        <v>1623000</v>
-      </c>
-      <c r="E37" s="1">
-        <v>2912000</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>7</v>
-      </c>
-      <c r="B38" t="s">
-        <v>188</v>
-      </c>
-      <c r="C38" t="s">
-        <v>187</v>
-      </c>
-      <c r="D38" s="1">
-        <v>1408000</v>
-      </c>
-      <c r="E38" s="1">
-        <v>2705000</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>8</v>
-      </c>
-      <c r="B39" t="s">
-        <v>189</v>
       </c>
       <c r="C39" t="s">
         <v>187</v>
       </c>
       <c r="D39" s="1">
-        <v>1251000</v>
+        <v>1623000</v>
       </c>
       <c r="E39" s="1">
-        <v>2396000</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2912000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C40" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="D40" s="1">
-        <v>1115000</v>
+        <v>1408000</v>
       </c>
       <c r="E40" s="1">
-        <v>1958000</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2705000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C41" t="s">
         <v>187</v>
       </c>
       <c r="D41" s="1">
+        <v>1251000</v>
+      </c>
+      <c r="E41" s="1">
+        <v>2396000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42">
+        <v>9</v>
+      </c>
+      <c r="B42" t="s">
+        <v>190</v>
+      </c>
+      <c r="C42" t="s">
+        <v>181</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1115000</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1958000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43">
+        <v>10</v>
+      </c>
+      <c r="B43" t="s">
+        <v>191</v>
+      </c>
+      <c r="C43" t="s">
+        <v>187</v>
+      </c>
+      <c r="D43" s="1">
         <v>1059000</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E43" s="1">
         <v>1403000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added text to land grant
</commit_message>
<xml_diff>
--- a/obsidian-notes/spreadsheets/area.xlsx
+++ b/obsidian-notes/spreadsheets/area.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sharm\iCloudDrive\iCloud~md~obsidian\Ishan's notes\Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0B0CA0-5B5B-4BCE-8D3D-9C47C09A2FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BB9342-8D54-4DBA-9217-A961931070A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" activeTab="2" xr2:uid="{94B94BC7-FBC8-4BAC-A974-CA3E4662C848}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <sheet name="buenaventura" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2056,10 +2057,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C745E12-030D-4421-A6DC-982053D4A77E}">
-  <dimension ref="A1:L259"/>
+  <dimension ref="A1:M259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="I247" sqref="I247"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2469,7 +2470,7 @@
       </c>
       <c r="B34" s="12">
         <f>C84^(1/3)</f>
-        <v>683.35638761533869</v>
+        <v>681.49541140077338</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -2486,7 +2487,7 @@
       </c>
       <c r="B36" s="15">
         <f>C84/B35</f>
-        <v>460477.63347763347</v>
+        <v>456725.82972582971</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -2495,7 +2496,7 @@
       </c>
       <c r="B37" s="15">
         <f>B36+C37</f>
-        <v>462477.63347763347</v>
+        <v>458725.82972582971</v>
       </c>
       <c r="C37">
         <v>2000</v>
@@ -2548,7 +2549,7 @@
       <c r="D41" s="23"/>
       <c r="E41" s="24">
         <f t="shared" ref="E41:E82" si="0">C41/$B$37</f>
-        <v>3.2844831620888808</v>
+        <v>3.3113461278338581</v>
       </c>
       <c r="F41" s="25">
         <f t="shared" ref="F41:F83" si="1">FLOOR(E41,1)</f>
@@ -2586,15 +2587,15 @@
       <c r="D42" s="1"/>
       <c r="E42" s="12">
         <f t="shared" si="0"/>
-        <v>33.804878048780488</v>
+        <v>34.081359685684355</v>
       </c>
       <c r="F42" s="15">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G42">
         <f t="shared" ref="G42:G83" si="3">SQRT(F42*(F42+1))</f>
-        <v>33.496268448888451</v>
+        <v>34.496376621320678</v>
       </c>
       <c r="H42">
         <f t="shared" si="2"/>
@@ -2622,7 +2623,7 @@
       <c r="D43" s="23"/>
       <c r="E43" s="24">
         <f t="shared" si="0"/>
-        <v>23.000031201540107</v>
+        <v>23.188142700308592</v>
       </c>
       <c r="F43" s="25">
         <f t="shared" si="1"/>
@@ -2660,15 +2661,15 @@
       <c r="D44" s="1"/>
       <c r="E44" s="12">
         <f t="shared" si="0"/>
-        <v>25.970985687853553</v>
+        <v>26.183395879797544</v>
       </c>
       <c r="F44" s="15">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G44">
         <f t="shared" si="3"/>
-        <v>25.495097567963924</v>
+        <v>26.49528259898354</v>
       </c>
       <c r="H44">
         <f t="shared" si="2"/>
@@ -2696,7 +2697,7 @@
       <c r="D45" s="23"/>
       <c r="E45" s="24">
         <f t="shared" si="0"/>
-        <v>7.8836244957051083</v>
+        <v>7.9481026873484177</v>
       </c>
       <c r="F45" s="25">
         <f t="shared" si="1"/>
@@ -2734,7 +2735,7 @@
       <c r="D46" s="1"/>
       <c r="E46" s="12">
         <f t="shared" si="0"/>
-        <v>18.77496201212492</v>
+        <v>18.92851772744002</v>
       </c>
       <c r="F46" s="15">
         <f t="shared" si="1"/>
@@ -2770,7 +2771,7 @@
       <c r="D47" s="23"/>
       <c r="E47" s="24">
         <f t="shared" si="0"/>
-        <v>10.329148166753511</v>
+        <v>10.413627684438671</v>
       </c>
       <c r="F47" s="25">
         <f t="shared" si="1"/>
@@ -2808,7 +2809,7 @@
       <c r="D48" s="1"/>
       <c r="E48" s="12">
         <f t="shared" si="0"/>
-        <v>19.499321366502652</v>
+        <v>19.658801435685145</v>
       </c>
       <c r="F48" s="15">
         <f t="shared" si="1"/>
@@ -2844,7 +2845,7 @@
       <c r="D49" s="23"/>
       <c r="E49" s="24">
         <f t="shared" si="0"/>
-        <v>3.7709931762231785</v>
+        <v>3.8018351856104338</v>
       </c>
       <c r="F49" s="25">
         <f t="shared" si="1"/>
@@ -2882,7 +2883,7 @@
       <c r="D50" s="1"/>
       <c r="E50" s="12">
         <f t="shared" si="0"/>
-        <v>41.387947469087074</v>
+        <v>41.726449132895247</v>
       </c>
       <c r="F50" s="15">
         <f t="shared" si="1"/>
@@ -2894,7 +2895,7 @@
       </c>
       <c r="H50">
         <f t="shared" si="2"/>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K50" s="11">
         <f>K127+K129*(2.5/9)</f>
@@ -2913,24 +2914,24 @@
         <v>87</v>
       </c>
       <c r="C51" s="23">
-        <v>39239000</v>
+        <v>36239000</v>
       </c>
       <c r="D51" s="23"/>
       <c r="E51" s="24">
         <f t="shared" si="0"/>
-        <v>84.845184198292031</v>
+        <v>78.999257621179183</v>
       </c>
       <c r="F51" s="25">
         <f t="shared" si="1"/>
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="G51" s="22">
         <f t="shared" si="3"/>
-        <v>84.498520697110436</v>
+        <v>78.498407627161455</v>
       </c>
       <c r="H51" s="22">
         <f t="shared" si="2"/>
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I51" s="22"/>
       <c r="J51" s="22"/>
@@ -2956,7 +2957,7 @@
       <c r="D52" s="1"/>
       <c r="E52" s="12">
         <f t="shared" si="0"/>
-        <v>27.052119052596435</v>
+        <v>27.273371563745492</v>
       </c>
       <c r="F52" s="15">
         <f t="shared" si="1"/>
@@ -2992,7 +2993,7 @@
       <c r="D53" s="23"/>
       <c r="E53" s="24">
         <f t="shared" si="0"/>
-        <v>2.3741688689753726</v>
+        <v>2.3935866019496883</v>
       </c>
       <c r="F53" s="25">
         <f t="shared" si="1"/>
@@ -3030,7 +3031,7 @@
       <c r="D54" s="1"/>
       <c r="E54" s="12">
         <f t="shared" si="0"/>
-        <v>1.8314399198744451</v>
+        <v>1.8464188086078195</v>
       </c>
       <c r="F54" s="15">
         <f t="shared" si="1"/>
@@ -3058,7 +3059,7 @@
       <c r="D55" s="23"/>
       <c r="E55" s="24">
         <f t="shared" si="0"/>
-        <v>20.370714858485414</v>
+        <v>20.537321836947189</v>
       </c>
       <c r="F55" s="25">
         <f t="shared" si="1"/>
@@ -3070,7 +3071,7 @@
       </c>
       <c r="H55" s="22">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I55" s="22"/>
       <c r="J55" s="22"/>
@@ -3097,7 +3098,7 @@
       <c r="D56" s="1"/>
       <c r="E56" s="12">
         <f t="shared" si="0"/>
-        <v>22.660555325010844</v>
+        <v>22.845890335548937</v>
       </c>
       <c r="F56" s="15">
         <f t="shared" si="1"/>
@@ -3133,15 +3134,15 @@
       <c r="D57" s="23"/>
       <c r="E57" s="24">
         <f t="shared" si="0"/>
-        <v>50.71812840681816</v>
+        <v>51.132939285366014</v>
       </c>
       <c r="F57" s="25">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G57" s="22">
         <f t="shared" si="3"/>
-        <v>50.497524691810391</v>
+        <v>51.497572758334933</v>
       </c>
       <c r="H57" s="22">
         <f t="shared" si="2"/>
@@ -3171,7 +3172,7 @@
       <c r="D58" s="1"/>
       <c r="E58" s="12">
         <f t="shared" si="0"/>
-        <v>19.680951771779455</v>
+        <v>19.8419173505884</v>
       </c>
       <c r="F58" s="15">
         <f t="shared" si="1"/>
@@ -3207,7 +3208,7 @@
       <c r="D59" s="23"/>
       <c r="E59" s="24">
         <f t="shared" si="0"/>
-        <v>11.680564872682115</v>
+        <v>11.776097289373602</v>
       </c>
       <c r="F59" s="25">
         <f t="shared" si="1"/>
@@ -3245,15 +3246,15 @@
       <c r="D60" s="1"/>
       <c r="E60" s="12">
         <f t="shared" si="0"/>
-        <v>14.926127233640253</v>
+        <v>15.048204292585336</v>
       </c>
       <c r="F60" s="15">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G60">
         <f t="shared" si="3"/>
-        <v>14.491376746189438</v>
+        <v>15.491933384829668</v>
       </c>
       <c r="H60">
         <f t="shared" si="2"/>
@@ -3281,7 +3282,7 @@
       <c r="D61" s="23"/>
       <c r="E61" s="24">
         <f t="shared" si="0"/>
-        <v>3.2455623609581368</v>
+        <v>3.2721070032117323</v>
       </c>
       <c r="F61" s="25">
         <f t="shared" si="1"/>
@@ -3319,7 +3320,7 @@
       <c r="D62" s="1"/>
       <c r="E62" s="12">
         <f t="shared" si="0"/>
-        <v>25.110403529518216</v>
+        <v>25.315775235374982</v>
       </c>
       <c r="F62" s="15">
         <f t="shared" si="1"/>
@@ -3355,7 +3356,7 @@
       <c r="D63" s="23"/>
       <c r="E63" s="24">
         <f t="shared" si="0"/>
-        <v>19.203090824563102</v>
+        <v>19.360148098283407</v>
       </c>
       <c r="F63" s="25">
         <f t="shared" si="1"/>
@@ -3393,7 +3394,7 @@
       <c r="D64" s="1"/>
       <c r="E64" s="12">
         <f t="shared" si="0"/>
-        <v>48.008808194772492</v>
+        <v>48.401460221392462</v>
       </c>
       <c r="F64" s="15">
         <f t="shared" si="1"/>
@@ -3429,7 +3430,7 @@
       <c r="D65" s="23"/>
       <c r="E65" s="24">
         <f t="shared" si="0"/>
-        <v>15.771573524869188</v>
+        <v>15.900565277432628</v>
       </c>
       <c r="F65" s="25">
         <f t="shared" si="1"/>
@@ -3467,7 +3468,7 @@
       <c r="D66" s="1"/>
       <c r="E66" s="12">
         <f t="shared" si="0"/>
-        <v>7.6241524881668159</v>
+        <v>7.6865085232009109</v>
       </c>
       <c r="F66" s="15">
         <f t="shared" si="1"/>
@@ -3503,7 +3504,7 @@
       <c r="D67" s="23"/>
       <c r="E67" s="24">
         <f t="shared" si="0"/>
-        <v>19.594461102600025</v>
+        <v>19.754719295872562</v>
       </c>
       <c r="F67" s="25">
         <f t="shared" si="1"/>
@@ -3536,24 +3537,24 @@
         <v>232</v>
       </c>
       <c r="C68" s="1">
-        <v>3443000</v>
+        <v>3943000</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="12">
         <f t="shared" si="0"/>
-        <v>7.4446843496194974</v>
+        <v>8.5955482436134982</v>
       </c>
       <c r="F68" s="15">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G68">
         <f t="shared" si="3"/>
-        <v>7.4833147735478827</v>
+        <v>8.4852813742385695</v>
       </c>
       <c r="H68">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K68" s="11">
         <f>K131*(1/3)</f>
@@ -3572,12 +3573,12 @@
         <v>104</v>
       </c>
       <c r="C69" s="23">
-        <v>5337000</v>
+        <v>5137000</v>
       </c>
       <c r="D69" s="23"/>
       <c r="E69" s="24">
         <f t="shared" si="0"/>
-        <v>11.540017535265541</v>
+        <v>11.198410176881191</v>
       </c>
       <c r="F69" s="25">
         <f t="shared" si="1"/>
@@ -3589,7 +3590,7 @@
       </c>
       <c r="H69" s="22">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I69" s="22"/>
       <c r="J69" s="22"/>
@@ -3615,7 +3616,7 @@
       <c r="D70" s="1"/>
       <c r="E70" s="12">
         <f t="shared" si="0"/>
-        <v>4.181823854825474</v>
+        <v>4.216025945510653</v>
       </c>
       <c r="F70" s="15">
         <f t="shared" si="1"/>
@@ -3642,12 +3643,12 @@
         <v>195</v>
       </c>
       <c r="C71" s="23">
-        <v>8321000</v>
+        <v>7821000</v>
       </c>
       <c r="D71" s="23"/>
       <c r="E71" s="24">
         <f t="shared" si="0"/>
-        <v>17.99222145605107</v>
+        <v>17.049399648313763</v>
       </c>
       <c r="F71" s="25">
         <f t="shared" si="1"/>
@@ -3659,7 +3660,7 @@
       </c>
       <c r="H71" s="22">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I71" s="22"/>
       <c r="J71" s="22"/>
@@ -3685,7 +3686,7 @@
       <c r="D72" s="1"/>
       <c r="E72" s="12">
         <f t="shared" si="0"/>
-        <v>1.8854965881115893</v>
+        <v>1.9009175928052169</v>
       </c>
       <c r="F72" s="15">
         <f t="shared" si="1"/>
@@ -3713,7 +3714,7 @@
       <c r="D73" s="23"/>
       <c r="E73" s="24">
         <f t="shared" si="0"/>
-        <v>10.621054175234089</v>
+        <v>10.707921119104617</v>
       </c>
       <c r="F73" s="25">
         <f t="shared" si="1"/>
@@ -3746,20 +3747,20 @@
         <v>226</v>
       </c>
       <c r="C74" s="1">
-        <v>1683000</v>
+        <v>1883000</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="12">
         <f t="shared" si="0"/>
-        <v>3.6390949057245465</v>
+        <v>4.1048484257479627</v>
       </c>
       <c r="F74" s="15">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G74">
         <f t="shared" si="3"/>
-        <v>3.4641016151377544</v>
+        <v>4.4721359549995796</v>
       </c>
       <c r="H74">
         <f t="shared" si="2"/>
@@ -3783,7 +3784,7 @@
       <c r="D75" s="23"/>
       <c r="E75" s="24">
         <f t="shared" si="0"/>
-        <v>7.4079258152182392</v>
+        <v>7.4685133864113222</v>
       </c>
       <c r="F75" s="25">
         <f t="shared" si="1"/>
@@ -3813,24 +3814,24 @@
         <v>114</v>
       </c>
       <c r="C76" s="1">
-        <v>7804000</v>
+        <v>8304000</v>
       </c>
       <c r="D76" s="1"/>
       <c r="E76" s="12">
         <f t="shared" si="0"/>
-        <v>16.874329556906929</v>
+        <v>18.102316159007479</v>
       </c>
       <c r="F76" s="15">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G76">
         <f t="shared" si="3"/>
-        <v>16.492422502470642</v>
+        <v>18.493242008906929</v>
       </c>
       <c r="H76">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L76" s="1">
         <f>E219+E250</f>
@@ -3845,24 +3846,24 @@
         <v>115</v>
       </c>
       <c r="C77" s="23">
-        <v>2701000</v>
+        <v>3101000</v>
       </c>
       <c r="D77" s="23"/>
       <c r="E77" s="24">
         <f t="shared" si="0"/>
-        <v>5.8402824363410577</v>
+        <v>6.7600291918451578</v>
       </c>
       <c r="F77" s="25">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G77" s="22">
         <f t="shared" si="3"/>
-        <v>5.4772255750516612</v>
+        <v>6.4807406984078604</v>
       </c>
       <c r="H77" s="22">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I77" s="22"/>
       <c r="J77" s="22"/>
@@ -3871,8 +3872,8 @@
         <v>1648666.6666666665</v>
       </c>
       <c r="L77" s="23">
-        <f>E234*(2/3)</f>
-        <v>1648666.6666666665</v>
+        <f>E234*(2/3)+E259</f>
+        <v>2387666.6666666665</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -3888,7 +3889,7 @@
       <c r="D78" s="1"/>
       <c r="E78" s="12">
         <f t="shared" si="0"/>
-        <v>2.3093008670907995</v>
+        <v>2.3281880609128116</v>
       </c>
       <c r="F78" s="15">
         <f t="shared" si="1"/>
@@ -3917,7 +3918,7 @@
       <c r="D79" s="23"/>
       <c r="E79" s="24">
         <f t="shared" si="0"/>
-        <v>7.6371260885437309</v>
+        <v>7.6995882314082866</v>
       </c>
       <c r="F79" s="25">
         <f t="shared" si="1"/>
@@ -3955,7 +3956,7 @@
       <c r="D80" s="1"/>
       <c r="E80" s="12">
         <f t="shared" si="0"/>
-        <v>2.2292969980998261</v>
+        <v>2.2475298603006637</v>
       </c>
       <c r="F80" s="15">
         <f t="shared" si="1"/>
@@ -3970,7 +3971,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="22">
         <v>41</v>
       </c>
@@ -3978,30 +3979,30 @@
         <v>112</v>
       </c>
       <c r="C81" s="23">
-        <v>3121000</v>
+        <v>2621000</v>
       </c>
       <c r="D81" s="23"/>
       <c r="E81" s="24">
         <f>C81/$B$37</f>
-        <v>6.7484344627250801</v>
+        <v>5.7136525352551297</v>
       </c>
       <c r="F81" s="25">
         <f>FLOOR(E81,1)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G81" s="22">
         <f>SQRT(F81*(F81+1))</f>
-        <v>6.4807406984078604</v>
+        <v>5.4772255750516612</v>
       </c>
       <c r="H81" s="22">
         <f>IF(E81&gt;G81,CEILING(E81,1),FLOOR(E81,1))</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I81" s="22"/>
       <c r="J81" s="22"/>
       <c r="K81" s="22"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A82">
         <v>42</v>
       </c>
@@ -4014,7 +4015,7 @@
       <c r="D82" s="1"/>
       <c r="E82" s="12">
         <f t="shared" si="0"/>
-        <v>0.83247269085202047</v>
+        <v>0.83928127663991803</v>
       </c>
       <c r="F82" s="15">
         <f t="shared" si="1"/>
@@ -4029,7 +4030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="22">
         <v>43</v>
       </c>
@@ -4042,7 +4043,7 @@
       <c r="D83" s="23"/>
       <c r="E83" s="24">
         <f>C83/$B$37</f>
-        <v>0.41515521206126738</v>
+        <v>0.41855066263601104</v>
       </c>
       <c r="F83" s="25">
         <f t="shared" si="1"/>
@@ -4060,49 +4061,52 @@
       <c r="J83" s="22"/>
       <c r="K83" s="22"/>
     </row>
-    <row r="84" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="84" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A84" s="4"/>
       <c r="B84" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C84" s="7">
         <f>SUM(C41:C83)</f>
-        <v>319111000</v>
+        <v>316511000</v>
       </c>
       <c r="D84" s="7"/>
       <c r="E84" s="7">
         <f>SUM(E41:E83)</f>
-        <v>690.00309831293259</v>
+        <v>689.97858740409629</v>
       </c>
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
       <c r="H84" s="7">
         <f>SUM(H41:H83)</f>
-        <v>693</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
         <v>64</v>
       </c>
       <c r="B86" s="12">
         <f>$C$84/B32</f>
-        <v>74.34052833172214</v>
+        <v>73.734828830098948</v>
       </c>
       <c r="C86" s="12">
         <f>$C$84/C32</f>
-        <v>69.113612817381039</v>
+        <v>68.550500316322811</v>
       </c>
       <c r="I86" s="1"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="J87" s="1">
         <f>C80+C82+C83</f>
         <v>1608000</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="M88" s="15"/>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
         <v>250</v>
       </c>
@@ -4113,7 +4117,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
         <v>251</v>
       </c>
@@ -4122,10 +4126,10 @@
       </c>
       <c r="C91" s="1">
         <f>C46+C49+C53+C54+C72+C45+C51</f>
-        <v>56129000</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>53129000</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
         <v>252</v>
       </c>
@@ -4137,7 +4141,7 @@
         <v>55240000</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
         <v>253</v>
       </c>
@@ -4150,7 +4154,7 @@
       </c>
       <c r="J93" s="1"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
         <v>254</v>
       </c>
@@ -4159,10 +4163,10 @@
       </c>
       <c r="C94" s="1">
         <f>C52+C48+C75+C44+C77+C67+C61+C59</f>
-        <v>55632000</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>56032000</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
         <v>255</v>
       </c>
@@ -4171,11 +4175,11 @@
       </c>
       <c r="C95" s="1">
         <f>C56+C55+C60+C64+C68</f>
-        <v>52450000</v>
+        <v>52950000</v>
       </c>
       <c r="J95" s="15"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
         <v>256</v>
       </c>
@@ -4184,7 +4188,7 @@
       </c>
       <c r="C96" s="1">
         <f>C66+C62+C76+C71+C70+C81+C78+C83+C82+C80</f>
-        <v>38995000</v>
+        <v>38495000</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -4202,7 +4206,7 @@
     <row r="98" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C98" s="1">
         <f>SUM(C91:C97)</f>
-        <v>319111000</v>
+        <v>316511000</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Updated sheysh and frep
</commit_message>
<xml_diff>
--- a/obsidian-notes/spreadsheets/area.xlsx
+++ b/obsidian-notes/spreadsheets/area.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sharm\iCloudDrive\iCloud~md~obsidian\Ishan's notes\Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1CA619-8B95-4E17-8449-2A093B69DA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F949633-8560-44CF-99CA-0B16BE2C1259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" activeTab="2" xr2:uid="{94B94BC7-FBC8-4BAC-A974-CA3E4662C848}"/>
   </bookViews>
@@ -980,7 +980,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1011,7 +1011,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1347,10 +1346,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="33"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
@@ -1914,11 +1913,11 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="34" t="s">
+      <c r="A55" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="B55" s="34"/>
-      <c r="C55" s="34"/>
+      <c r="B55" s="33"/>
+      <c r="C55" s="33"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
@@ -2082,8 +2081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C745E12-030D-4421-A6DC-982053D4A77E}">
   <dimension ref="A1:N319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" zoomScale="93" workbookViewId="0">
-      <selection activeCell="K132" sqref="K132"/>
+    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="93" workbookViewId="0">
+      <selection activeCell="F147" sqref="F147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4260,7 +4259,7 @@
       <c r="F101" s="28">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="G101" s="16">
+      <c r="G101" s="28">
         <f>SUM(B101:F101)</f>
         <v>1</v>
       </c>
@@ -4290,13 +4289,13 @@
         <v>78</v>
       </c>
       <c r="B102" s="28">
-        <v>0.90400000000000003</v>
+        <v>0.85399999999999998</v>
       </c>
       <c r="C102" s="28">
-        <v>5.3999999999999999E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="D102" s="28">
-        <v>3.5999999999999997E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="E102" s="28">
         <v>1E-3</v>
@@ -4304,21 +4303,21 @@
       <c r="F102" s="28">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G102" s="16">
+      <c r="G102" s="28">
         <f t="shared" ref="G102:G143" si="5">SUM(B102:F102)</f>
         <v>1</v>
       </c>
       <c r="I102" s="11">
         <f t="shared" ref="I102:I143" si="6">B102*$C42</f>
-        <v>14133136</v>
+        <v>13351436</v>
       </c>
       <c r="J102" s="11">
         <f t="shared" si="4"/>
-        <v>844236</v>
+        <v>1313256</v>
       </c>
       <c r="K102" s="11">
         <f t="shared" si="4"/>
-        <v>562824</v>
+        <v>875504</v>
       </c>
       <c r="L102" s="11">
         <f t="shared" si="4"/>
@@ -4348,7 +4347,7 @@
       <c r="F103" s="28">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="G103" s="16">
+      <c r="G103" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -4378,13 +4377,13 @@
         <v>80</v>
       </c>
       <c r="B104" s="28">
-        <v>0.441</v>
+        <v>0.43099999999999999</v>
       </c>
       <c r="C104" s="28">
         <v>0.51400000000000001</v>
       </c>
       <c r="D104" s="28">
-        <v>3.5999999999999997E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="E104" s="28">
         <v>2E-3</v>
@@ -4392,13 +4391,13 @@
       <c r="F104" s="28">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="G104" s="16">
+      <c r="G104" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I104" s="11">
         <f t="shared" si="6"/>
-        <v>5296851</v>
+        <v>5176741</v>
       </c>
       <c r="J104" s="11">
         <f t="shared" si="4"/>
@@ -4406,7 +4405,7 @@
       </c>
       <c r="K104" s="11">
         <f t="shared" si="4"/>
-        <v>432395.99999999994</v>
+        <v>552506</v>
       </c>
       <c r="L104" s="11">
         <f t="shared" si="4"/>
@@ -4436,7 +4435,7 @@
       <c r="F105" s="28">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G105" s="16">
+      <c r="G105" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -4480,7 +4479,7 @@
       <c r="F106" s="28">
         <v>1.4E-2</v>
       </c>
-      <c r="G106" s="16">
+      <c r="G106" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -4524,7 +4523,7 @@
       <c r="F107" s="28">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="G107" s="16">
+      <c r="G107" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -4568,7 +4567,7 @@
       <c r="F108" s="28">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="G108" s="16">
+      <c r="G108" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -4612,7 +4611,7 @@
       <c r="F109" s="28">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G109" s="16">
+      <c r="G109" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -4656,7 +4655,7 @@
       <c r="F110" s="28">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="G110" s="16">
+      <c r="G110" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -4686,27 +4685,27 @@
         <v>87</v>
       </c>
       <c r="B111" s="28">
-        <v>0.78700000000000003</v>
+        <v>0.78200000000000003</v>
       </c>
       <c r="C111" s="28">
         <v>0.11899999999999999</v>
       </c>
       <c r="D111" s="28">
-        <v>6.6000000000000003E-2</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="E111" s="28">
-        <v>6.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="F111" s="28">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="G111" s="16">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="G111" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I111" s="11">
         <f t="shared" si="6"/>
-        <v>28520093</v>
+        <v>28338898</v>
       </c>
       <c r="J111" s="11">
         <f t="shared" si="4"/>
@@ -4714,15 +4713,15 @@
       </c>
       <c r="K111" s="11">
         <f t="shared" si="4"/>
-        <v>2391774</v>
+        <v>2862881</v>
       </c>
       <c r="L111" s="11">
         <f t="shared" si="4"/>
-        <v>217434</v>
+        <v>108717</v>
       </c>
       <c r="M111" s="11">
         <f t="shared" si="4"/>
-        <v>797258</v>
+        <v>616063</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4744,7 +4743,7 @@
       <c r="F112" s="28">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="G112" s="16">
+      <c r="G112" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -4788,7 +4787,7 @@
       <c r="F113" s="28">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="G113" s="16">
+      <c r="G113" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -4832,7 +4831,7 @@
       <c r="F114" s="28">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G114" s="16">
+      <c r="G114" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -4876,7 +4875,7 @@
       <c r="F115" s="28">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="G115" s="16">
+      <c r="G115" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -4920,7 +4919,7 @@
       <c r="F116" s="28">
         <v>1.6E-2</v>
       </c>
-      <c r="G116" s="16">
+      <c r="G116" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -4953,18 +4952,18 @@
         <v>0.81100000000000005</v>
       </c>
       <c r="C117" s="28">
-        <v>6.9000000000000006E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="D117" s="28">
-        <v>9.7000000000000003E-2</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="E117" s="28">
         <v>2E-3</v>
       </c>
       <c r="F117" s="28">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="G117" s="16">
+        <v>1.6E-2</v>
+      </c>
+      <c r="G117" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -4974,11 +4973,11 @@
       </c>
       <c r="J117" s="11">
         <f t="shared" ref="J117:J143" si="7">C117*$C57</f>
-        <v>1618464.0000000002</v>
+        <v>1688831.9999999998</v>
       </c>
       <c r="K117" s="11">
         <f t="shared" ref="K117:K143" si="8">D117*$C57</f>
-        <v>2275232</v>
+        <v>2322144</v>
       </c>
       <c r="L117" s="11">
         <f t="shared" ref="L117:L143" si="9">E117*$C57</f>
@@ -4986,7 +4985,7 @@
       </c>
       <c r="M117" s="11">
         <f t="shared" ref="M117:M143" si="10">F117*$C57</f>
-        <v>492576.00000000006</v>
+        <v>375296</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5008,7 +5007,7 @@
       <c r="F118" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="G118" s="16">
+      <c r="G118" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -5052,7 +5051,7 @@
       <c r="F119" s="28">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="G119" s="16">
+      <c r="G119" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -5096,7 +5095,7 @@
       <c r="F120" s="28">
         <v>1.4E-2</v>
       </c>
-      <c r="G120" s="16">
+      <c r="G120" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -5126,10 +5125,10 @@
         <v>97</v>
       </c>
       <c r="B121" s="28">
-        <v>0.41199999999999998</v>
+        <v>0.40200000000000002</v>
       </c>
       <c r="C121" s="28">
-        <v>0.57099999999999995</v>
+        <v>0.58099999999999996</v>
       </c>
       <c r="D121" s="28">
         <v>3.0000000000000001E-3</v>
@@ -5140,17 +5139,17 @@
       <c r="F121" s="28">
         <v>1.2E-2</v>
       </c>
-      <c r="G121" s="16">
+      <c r="G121" s="28">
         <f t="shared" si="5"/>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="I121" s="11">
         <f t="shared" si="6"/>
-        <v>618412</v>
+        <v>603402</v>
       </c>
       <c r="J121" s="11">
         <f t="shared" si="7"/>
-        <v>857070.99999999988</v>
+        <v>872080.99999999988</v>
       </c>
       <c r="K121" s="11">
         <f t="shared" si="8"/>
@@ -5170,7 +5169,7 @@
         <v>98</v>
       </c>
       <c r="B122" s="28">
-        <v>0.30099999999999999</v>
+        <v>0.30499999999999999</v>
       </c>
       <c r="C122" s="28">
         <v>0.55700000000000005</v>
@@ -5179,18 +5178,18 @@
         <v>9.0999999999999998E-2</v>
       </c>
       <c r="E122" s="28">
-        <v>8.9999999999999993E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="F122" s="28">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="G122" s="16">
+      <c r="G122" s="28">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0.99900000000000011</v>
       </c>
       <c r="I122" s="11">
         <f t="shared" si="6"/>
-        <v>3495513</v>
+        <v>3541965</v>
       </c>
       <c r="J122" s="11">
         <f t="shared" si="7"/>
@@ -5201,8 +5200,8 @@
         <v>1056783</v>
       </c>
       <c r="L122" s="11">
-        <f t="shared" si="9"/>
-        <v>104516.99999999999</v>
+        <f>E122*$C62</f>
+        <v>46452</v>
       </c>
       <c r="M122" s="11">
         <f t="shared" si="10"/>
@@ -5228,7 +5227,7 @@
       <c r="F123" s="28">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="G123" s="16">
+      <c r="G123" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -5272,7 +5271,7 @@
       <c r="F124" s="28">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="G124" s="16">
+      <c r="G124" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -5316,7 +5315,7 @@
       <c r="F125" s="28">
         <v>1.4E-2</v>
       </c>
-      <c r="G125" s="16">
+      <c r="G125" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -5360,7 +5359,7 @@
       <c r="F126" s="28">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="G126" s="16">
+      <c r="G126" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -5404,7 +5403,7 @@
       <c r="F127" s="28">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="G127" s="16">
+      <c r="G127" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -5448,7 +5447,7 @@
       <c r="F128" s="28">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="G128" s="16">
+      <c r="G128" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -5492,7 +5491,7 @@
       <c r="F129" s="28">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="G129" s="16">
+      <c r="G129" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -5536,7 +5535,7 @@
       <c r="F130" s="28">
         <v>1.9E-2</v>
       </c>
-      <c r="G130" s="16">
+      <c r="G130" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -5580,7 +5579,7 @@
       <c r="F131" s="28">
         <v>1.6E-2</v>
       </c>
-      <c r="G131" s="16">
+      <c r="G131" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -5624,7 +5623,7 @@
       <c r="F132" s="28">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="G132" s="16">
+      <c r="G132" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -5654,27 +5653,27 @@
         <v>38</v>
       </c>
       <c r="B133" s="28">
-        <v>0.55900000000000005</v>
+        <v>0.50900000000000001</v>
       </c>
       <c r="C133" s="28">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="D133" s="28">
-        <v>0.35399999999999998</v>
+        <v>0.41399999999999998</v>
       </c>
       <c r="E133" s="28">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="F133" s="28">
-        <v>6.2E-2</v>
-      </c>
-      <c r="G133" s="16">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="G133" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I133" s="11">
         <f t="shared" si="6"/>
-        <v>2745808.0000000005</v>
+        <v>2500208</v>
       </c>
       <c r="J133" s="11">
         <f t="shared" si="7"/>
@@ -5682,7 +5681,7 @@
       </c>
       <c r="K133" s="11">
         <f t="shared" si="8"/>
-        <v>1738848</v>
+        <v>2033568</v>
       </c>
       <c r="L133" s="11">
         <f t="shared" si="9"/>
@@ -5690,7 +5689,7 @@
       </c>
       <c r="M133" s="11">
         <f>F133*$C73</f>
-        <v>304544</v>
+        <v>255424</v>
       </c>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -5712,7 +5711,7 @@
       <c r="F134" s="28">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="G134" s="16">
+      <c r="G134" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -5756,7 +5755,7 @@
       <c r="F135" s="28">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="G135" s="16">
+      <c r="G135" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -5786,7 +5785,7 @@
         <v>114</v>
       </c>
       <c r="B136" s="28">
-        <v>0.69299999999999995</v>
+        <v>0.73299999999999998</v>
       </c>
       <c r="C136" s="28">
         <v>0.157</v>
@@ -5795,18 +5794,18 @@
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="E136" s="28">
-        <v>8.9999999999999993E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="F136" s="28">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="G136" s="16">
+        <v>1.4E-2</v>
+      </c>
+      <c r="G136" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I136" s="11">
         <f t="shared" si="6"/>
-        <v>5754672</v>
+        <v>6086832</v>
       </c>
       <c r="J136" s="11">
         <f t="shared" si="7"/>
@@ -5818,11 +5817,11 @@
       </c>
       <c r="L136" s="11">
         <f t="shared" si="9"/>
-        <v>74736</v>
+        <v>33216</v>
       </c>
       <c r="M136" s="11">
         <f t="shared" si="10"/>
-        <v>406896</v>
+        <v>116256</v>
       </c>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -5844,7 +5843,7 @@
       <c r="F137" s="28">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="G137" s="16">
+      <c r="G137" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -5880,15 +5879,15 @@
         <v>0.434</v>
       </c>
       <c r="D138" s="28">
-        <v>3.2000000000000001E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="E138" s="28">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="F138" s="28">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="G138" s="16">
+        <v>2.4E-2</v>
+      </c>
+      <c r="G138" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -5902,15 +5901,15 @@
       </c>
       <c r="K138" s="11">
         <f t="shared" si="8"/>
-        <v>34176</v>
+        <v>44856</v>
       </c>
       <c r="L138" s="11">
-        <f t="shared" si="9"/>
+        <f>E138*$C78</f>
         <v>8544</v>
       </c>
       <c r="M138" s="11">
-        <f t="shared" si="10"/>
-        <v>36312</v>
+        <f>F138*$C78</f>
+        <v>25632</v>
       </c>
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -5932,7 +5931,7 @@
       <c r="F139" s="28">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="G139" s="16">
+      <c r="G139" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -5976,7 +5975,7 @@
       <c r="F140" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="G140" s="16">
+      <c r="G140" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -6020,7 +6019,7 @@
       <c r="F141" s="28">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G141" s="16">
+      <c r="G141" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -6064,7 +6063,7 @@
       <c r="F142" s="28">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="G142" s="16">
+      <c r="G142" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -6077,7 +6076,7 @@
         <v>8085.0000000000009</v>
       </c>
       <c r="K142" s="11">
-        <f t="shared" si="8"/>
+        <f>D142*$C82</f>
         <v>58905</v>
       </c>
       <c r="L142" s="11">
@@ -6108,7 +6107,7 @@
       <c r="F143" s="29">
         <v>1.4E-2</v>
       </c>
-      <c r="G143" s="30">
+      <c r="G143" s="28">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -6125,7 +6124,7 @@
         <v>21888</v>
       </c>
       <c r="L143" s="10">
-        <f t="shared" si="9"/>
+        <f>E143*$C83</f>
         <v>45312</v>
       </c>
       <c r="M143" s="10">
@@ -6134,56 +6133,56 @@
       </c>
     </row>
     <row r="144" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A144" s="32" t="s">
+      <c r="A144" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B144" s="33">
+      <c r="B144" s="32">
         <f>I144/$N144</f>
-        <v>0.69952482907463498</v>
-      </c>
-      <c r="C144" s="33">
+        <v>0.69648324839234355</v>
+      </c>
+      <c r="C144" s="32">
         <f t="shared" ref="C144:G144" si="11">J144/$N144</f>
-        <v>0.21013793859718827</v>
-      </c>
-      <c r="D144" s="33">
+        <v>0.21190793038639963</v>
+      </c>
+      <c r="D144" s="32">
         <f t="shared" si="11"/>
-        <v>6.555121086039585E-2</v>
-      </c>
-      <c r="E144" s="33">
+        <v>6.9546673973652717E-2</v>
+      </c>
+      <c r="E144" s="32">
         <f t="shared" si="11"/>
-        <v>7.6216788351329105E-3</v>
-      </c>
-      <c r="F144" s="33">
+        <v>6.9598419147587215E-3</v>
+      </c>
+      <c r="F144" s="32">
         <f t="shared" si="11"/>
-        <v>1.7164342632647937E-2</v>
-      </c>
-      <c r="G144" s="33">
+        <v>1.510230533284542E-2</v>
+      </c>
+      <c r="G144" s="32">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="I144" s="31">
+      <c r="I144" s="30">
         <f>SUM(I101:I143)</f>
-        <v>220078206</v>
-      </c>
-      <c r="J144" s="31">
+        <v>219113203</v>
+      </c>
+      <c r="J144" s="30">
         <f t="shared" ref="J144:M144" si="12">SUM(J101:J143)</f>
-        <v>66111707</v>
-      </c>
-      <c r="K144" s="31">
+        <v>66666105</v>
+      </c>
+      <c r="K144" s="30">
         <f t="shared" si="12"/>
-        <v>20623132</v>
-      </c>
-      <c r="L144" s="31">
+        <v>21879341</v>
+      </c>
+      <c r="L144" s="30">
+        <f>SUM(L101:L143)</f>
+        <v>2189562</v>
+      </c>
+      <c r="M144" s="30">
         <f t="shared" si="12"/>
-        <v>2397864</v>
-      </c>
-      <c r="M144" s="31">
-        <f t="shared" si="12"/>
-        <v>5400091</v>
-      </c>
-      <c r="N144" s="31">
+        <v>4751176</v>
+      </c>
+      <c r="N144" s="30">
         <f>SUM(I144:M144)</f>
-        <v>314611000</v>
+        <v>314599387</v>
       </c>
     </row>
     <row r="145" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>